<commit_message>
Production underway, Mingze is tired
</commit_message>
<xml_diff>
--- a/hardware/Fabrication files/fydp-BOM-production.xlsx
+++ b/hardware/Fabrication files/fydp-BOM-production.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mingze\Documents\KiCad\7.0\projects\FYDP\hardware\Fabrication files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BFB555-71F5-40D4-8495-306034D48827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06369012-875E-4479-82B7-9B360DAAE528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="38610" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43605" yWindow="1605" windowWidth="19410" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fydp-BOM" sheetId="1" r:id="rId1"/>
@@ -307,9 +307,6 @@
     <t>J3</t>
   </si>
   <si>
-    <t>TerminalBlock_Phoenix:TerminalBlock_Phoenix_PT-1,5-2-3.5-H_1x02_P3.50mm_Horizontal</t>
-  </si>
-  <si>
     <t>C89122</t>
   </si>
   <si>
@@ -620,6 +617,9 @@
   </si>
   <si>
     <t>C137533</t>
+  </si>
+  <si>
+    <t>1751248:CONN_1751248_PXC</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1498,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,7 +1984,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1998,19 +1998,19 @@
         <v>1751248</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="H20" s="1">
         <v>1751248</v>
       </c>
       <c r="I20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2021,25 +2021,25 @@
         <v>4</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" s="3">
         <v>5011</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="H21" s="1">
         <v>5011</v>
       </c>
       <c r="I21" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2050,25 +2050,25 @@
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="J22" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2079,25 +2079,25 @@
         <v>2</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F23" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="J23" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2108,25 +2108,25 @@
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="J24" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2137,25 +2137,25 @@
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D25" s="3">
         <v>0</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="J25" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2166,25 +2166,25 @@
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="F26" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="J26" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2195,25 +2195,25 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="F27" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="J27" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2224,25 +2224,25 @@
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="F28" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="J28" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2253,25 +2253,25 @@
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="F29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="J29" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2282,25 +2282,25 @@
         <v>26</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="F30" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="J30" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2311,25 +2311,25 @@
         <v>43</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D31" s="3">
         <v>100</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="J31" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2340,25 +2340,25 @@
         <v>17</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="F32" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="J32" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2369,7 +2369,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D33" s="3">
         <v>0</v>
@@ -2378,19 +2378,19 @@
         <v>8</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="J33" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2401,25 +2401,25 @@
         <v>2</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="F34" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="J34" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2430,25 +2430,25 @@
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D35" s="3">
         <v>120</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="J35" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2459,25 +2459,25 @@
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D36" s="3">
         <v>290</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G36" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="J36" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2488,25 +2488,25 @@
         <v>2</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="F37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="J37" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2517,25 +2517,25 @@
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I38" s="3" t="s">
+      <c r="J38" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2546,25 +2546,25 @@
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="G39" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I39" s="3" t="s">
+      <c r="J39" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2575,25 +2575,25 @@
         <v>8</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="F40" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="I40" s="3" t="s">
+      <c r="J40" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>